<commit_message>
modifico el test y los graficos
</commit_message>
<xml_diff>
--- a/ComplejidadComputacional/Grafico.xlsx
+++ b/ComplejidadComputacional/Grafico.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximiliano\Documents\Maxi\TPs-Grupales\ComplejidadComputacional\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Polinomio" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Método</t>
   </si>
@@ -34,12 +29,6 @@
     <t>Gr 50</t>
   </si>
   <si>
-    <t>Gr 20</t>
-  </si>
-  <si>
-    <t>Gr 30</t>
-  </si>
-  <si>
     <t>evaluarHorner()(ns)</t>
   </si>
   <si>
@@ -47,12 +36,6 @@
   </si>
   <si>
     <t>resolverBinomio()(ns)</t>
-  </si>
-  <si>
-    <t>obtenerTerminosTarta()(ns)</t>
-  </si>
-  <si>
-    <t>resolverBinomioEstatico()(ns)</t>
   </si>
   <si>
     <t>evaluarProgDinamica()(ns)</t>
@@ -86,6 +69,9 @@
   </si>
   <si>
     <t>EvaluarPow()(ns)</t>
+  </si>
+  <si>
+    <t>Gr 70</t>
   </si>
 </sst>
 </file>
@@ -139,7 +125,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -202,11 +188,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -220,6 +232,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,7 +255,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-AR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -251,213 +266,389 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Gr 10</c:v>
+            <c:strRef>
+              <c:f>Polinomio!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EvaluarProgDinamica()(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Polinomio!$B$4:$B$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>EvaluarProgDinamica()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>EvaluarMejorada()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>EvaluarMSucesiva()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EvaluarRecursiva()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>EvaluarRecursivaPar()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>EvaluarHorner()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>EvaluarPow()(ns)</c:v>
+              <c:f>Polinomio!$C$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gr 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gr 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gr 100</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Polinomio!$C$4:$C$10</c:f>
+              <c:f>Polinomio!$C$4:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>11974</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13256</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15822</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10691</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14112</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7270</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>12402</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38914</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Gr 50</c:v>
+            <c:strRef>
+              <c:f>Polinomio!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EvaluarMejorada()(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Polinomio!$B$4:$B$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>EvaluarProgDinamica()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>EvaluarMejorada()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>EvaluarMSucesiva()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EvaluarRecursiva()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>EvaluarRecursivaPar()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>EvaluarHorner()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>EvaluarPow()(ns)</c:v>
+              <c:f>Polinomio!$C$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gr 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gr 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gr 100</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Polinomio!$D$4:$D$10</c:f>
+              <c:f>Polinomio!$C$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>12402</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>13256</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>14112</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>132139</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>53455</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>95790</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>18388</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>36349</c:v>
+                  <c:v>66283</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Gr 100</c:v>
+            <c:strRef>
+              <c:f>Polinomio!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EvaluarMSucesiva()(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Polinomio!$B$4:$B$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>EvaluarProgDinamica()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>EvaluarMejorada()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>EvaluarMSucesiva()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>EvaluarRecursiva()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>EvaluarRecursivaPar()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>EvaluarHorner()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>EvaluarPow()(ns)</c:v>
+              <c:f>Polinomio!$C$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gr 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gr 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gr 100</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Polinomio!$E$4:$E$10</c:f>
+              <c:f>Polinomio!$C$6:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>38914</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>66283</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>15822</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>132139</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>490070</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>659842</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1604060</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>51316</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>194147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Polinomio!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EvaluarRecursiva()(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Polinomio!$C$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gr 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gr 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gr 100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Polinomio!$C$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10691</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53455</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>659842</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Polinomio!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EvaluarRecursivaPar()(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Polinomio!$C$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gr 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gr 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gr 100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Polinomio!$C$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>14112</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95790</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1604060</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Polinomio!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EvaluarHorner()(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Polinomio!$C$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gr 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gr 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gr 100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Polinomio!$C$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7270</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18388</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51316</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Polinomio!$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EvaluarPow()(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Polinomio!$C$3:$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gr 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gr 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gr 100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Polinomio!$C$10:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12402</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36349</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>194147</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -467,22 +658,22 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="110193688"/>
-        <c:axId val="110196040"/>
-      </c:barChart>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="147454976"/>
+        <c:axId val="147550976"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="110193688"/>
+        <c:axId val="147454976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:axPos val="b"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110196040"/>
+        <c:crossAx val="147550976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -490,59 +681,31 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110196040"/>
+        <c:axId val="147550976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110193688"/>
+        <c:crossAx val="147454976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="lt1"/>
-    </a:solidFill>
-    <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1"/>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr>
-          <a:solidFill>
-            <a:schemeClr val="dk1"/>
-          </a:solidFill>
-          <a:latin typeface="+mn-lt"/>
-          <a:ea typeface="+mn-ea"/>
-          <a:cs typeface="+mn-cs"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -554,7 +717,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="es-AR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -581,14 +744,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Binomio!$B$5:$B$13</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>resolverBinomioEstatico()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>obtenerTerminosTarta()(ns)</c:v>
+              <c:f>Binomio!$B$5:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>evaluarRecursiva()(ns)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>evaluarMSucesivas()(ns)</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>resolverBinomio()(ns)</c:v>
@@ -604,48 +767,36 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>evaluarRecursivaPar()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>evaluarRecursiva()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>evaluarMSucesivas()(ns)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Binomio!$C$5:$C$13</c:f>
+              <c:f>Binomio!$C$5:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>175340</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10397</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>46789</c:v>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>65221</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29774</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50570</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109647</c:v>
+                  <c:v>21740</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>197080</c:v>
+                  <c:v>50097</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21267</c:v>
+                  <c:v>26466</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31192</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>71365</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>33555</c:v>
+                  <c:v>81290</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -655,19 +806,19 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Gr 20</c:v>
+            <c:v>Gr 50</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Binomio!$B$5:$B$13</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>resolverBinomioEstatico()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>obtenerTerminosTarta()(ns)</c:v>
+              <c:f>Binomio!$B$5:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>evaluarRecursiva()(ns)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>evaluarMSucesivas()(ns)</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>resolverBinomio()(ns)</c:v>
@@ -683,48 +834,36 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>evaluarRecursivaPar()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>evaluarRecursiva()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>evaluarMSucesivas()(ns)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Binomio!$D$5:$D$13</c:f>
+              <c:f>Binomio!$D$5:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>50570</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7562</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>54823</c:v>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>96886</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8507</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>397941</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7090</c:v>
+                  <c:v>7089</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>137059</c:v>
+                  <c:v>348317</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7562</c:v>
+                  <c:v>9925</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27412</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>88379</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9925</c:v>
+                  <c:v>101139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -734,19 +873,19 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Gr 30</c:v>
+            <c:v>Gr 70</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Binomio!$B$5:$B$13</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>resolverBinomioEstatico()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>obtenerTerminosTarta()(ns)</c:v>
+              <c:f>Binomio!$B$5:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>evaluarRecursiva()(ns)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>evaluarMSucesivas()(ns)</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>resolverBinomio()(ns)</c:v>
@@ -762,48 +901,36 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>evaluarRecursivaPar()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>evaluarRecursiva()(ns)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>evaluarMSucesivas()(ns)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Binomio!$E$5:$E$13</c:f>
+              <c:f>Binomio!$E$5:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>112955</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3520034</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>77036</c:v>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>119099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7089</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>787848</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7089</c:v>
+                  <c:v>6617</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>160216</c:v>
+                  <c:v>455601</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8979</c:v>
+                  <c:v>11815</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>83180</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>834638</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7561</c:v>
+                  <c:v>93105</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -818,11 +945,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="110197216"/>
-        <c:axId val="110197608"/>
+        <c:axId val="197962752"/>
+        <c:axId val="197985024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110197216"/>
+        <c:axId val="197962752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -832,7 +959,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110197608"/>
+        <c:crossAx val="197985024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -840,7 +967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110197608"/>
+        <c:axId val="197985024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -851,7 +978,469 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110197216"/>
+        <c:crossAx val="197962752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Binomio!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>evaluarRecursiva()(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Binomio!$C$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gr 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gr 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gr 70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Binomio!$C$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>65221</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96886</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>119099</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Binomio!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>evaluarMSucesivas()(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Binomio!$C$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gr 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gr 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gr 70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Binomio!$C$6:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>29774</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8507</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7089</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Binomio!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>resolverBinomio()(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Binomio!$C$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gr 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gr 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gr 70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Binomio!$C$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50570</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>397941</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>787848</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Binomio!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>evaluarPow()(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Binomio!$C$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gr 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gr 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gr 70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Binomio!$C$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>21740</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7089</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6617</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Binomio!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>evaluarHorner()(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Binomio!$C$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gr 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gr 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gr 70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Binomio!$C$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>348317</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>455601</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Binomio!$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>evaluarProgDinamica()(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Binomio!$C$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gr 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gr 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gr 70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Binomio!$C$10:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>26466</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9925</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11815</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Binomio!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>evaluarRecursivaPar()(ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Binomio!$C$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Gr 10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gr 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gr 70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Binomio!$C$11:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>81290</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101139</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>93105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="49633920"/>
+        <c:axId val="49664384"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="49633920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49664384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="49664384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49633920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -877,20 +1466,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>723899</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="3 Gráfico"/>
+        <xdr:cNvPr id="2" name="1 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -935,6 +1524,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="2 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -986,7 +1605,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1021,7 +1640,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1232,8 +1851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,7 +1882,7 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>11974</v>
@@ -1279,7 +1898,7 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>13256</v>
@@ -1295,7 +1914,7 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1">
         <v>15822</v>
@@ -1310,7 +1929,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1">
         <v>10691</v>
@@ -1326,7 +1945,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>14112</v>
@@ -1341,7 +1960,7 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1">
         <v>7270</v>
@@ -1356,7 +1975,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1">
         <v>12402</v>
@@ -1381,10 +2000,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:E13"/>
+  <dimension ref="B3:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,7 +2011,10 @@
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
@@ -1400,140 +2022,125 @@
         <v>1</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>65221</v>
+      </c>
+      <c r="D5" s="1">
+        <v>96886</v>
+      </c>
+      <c r="E5" s="1">
+        <v>119099</v>
+      </c>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <v>29774</v>
+      </c>
+      <c r="D6" s="1">
+        <v>8507</v>
+      </c>
+      <c r="E6" s="15">
+        <v>7089</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>50570</v>
+      </c>
+      <c r="D7" s="1">
+        <v>397941</v>
+      </c>
+      <c r="E7" s="1">
+        <v>787848</v>
+      </c>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>21740</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7089</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6617</v>
+      </c>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>5</v>
-      </c>
+      <c r="C9" s="1">
+        <v>50097</v>
+      </c>
+      <c r="D9" s="1">
+        <v>348317</v>
+      </c>
+      <c r="E9" s="1">
+        <v>455601</v>
+      </c>
+      <c r="F9" s="13"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1">
-        <v>175340</v>
-      </c>
-      <c r="D5" s="1">
-        <v>50570</v>
-      </c>
-      <c r="E5" s="1">
-        <v>112955</v>
-      </c>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <v>26466</v>
+      </c>
+      <c r="D10" s="1">
+        <v>9925</v>
+      </c>
+      <c r="E10" s="1">
+        <v>11815</v>
+      </c>
+      <c r="F10" s="13"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1">
-        <v>10397</v>
-      </c>
-      <c r="D6" s="1">
-        <v>7562</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3520034</v>
-      </c>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>81290</v>
+      </c>
+      <c r="D11" s="1">
+        <v>101139</v>
+      </c>
+      <c r="E11" s="1">
+        <v>93105</v>
+      </c>
+      <c r="F11" s="13"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1">
-        <v>46789</v>
-      </c>
-      <c r="D7" s="1">
-        <v>54823</v>
-      </c>
-      <c r="E7" s="1">
-        <v>77036</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1">
-        <v>109647</v>
-      </c>
-      <c r="D8" s="1">
-        <v>7090</v>
-      </c>
-      <c r="E8" s="1">
-        <v>7089</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1">
-        <v>197080</v>
-      </c>
-      <c r="D9" s="1">
-        <v>137059</v>
-      </c>
-      <c r="E9" s="1">
-        <v>160216</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1">
-        <v>21267</v>
-      </c>
-      <c r="D10" s="1">
-        <v>7562</v>
-      </c>
-      <c r="E10" s="1">
-        <v>8979</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1">
-        <v>31192</v>
-      </c>
-      <c r="D11" s="1">
-        <v>27412</v>
-      </c>
-      <c r="E11" s="1">
-        <v>83180</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="1">
-        <v>71365</v>
-      </c>
-      <c r="D12" s="1">
-        <v>88379</v>
-      </c>
-      <c r="E12" s="1">
-        <v>834638</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1">
-        <v>33555</v>
-      </c>
-      <c r="D13" s="1">
-        <v>9925</v>
-      </c>
-      <c r="E13" s="1">
-        <v>7561</v>
-      </c>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>